<commit_message>
Copy new version of data file from Box folder
</commit_message>
<xml_diff>
--- a/SecondaryMalignancies_Data_BG_3_4.xlsx
+++ b/SecondaryMalignancies_Data_BG_3_4.xlsx
@@ -220,6 +220,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">additional exposure, additional risk not accounted for CMF </t>
     </r>
@@ -269,6 +270,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>88% of planned</t>
     </r>
@@ -312,6 +314,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>0</t>
     </r>
@@ -339,6 +342,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Tailored</t>
     </r>
@@ -391,6 +395,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>CTCb</t>
     </r>
@@ -433,6 +438,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Lung: 1</t>
     </r>
@@ -583,6 +589,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>2</t>
     </r>
@@ -621,6 +628,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Impact of Tamoxifen on Endometrial CA</t>
     </r>
@@ -679,6 +687,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">86% of T at full dose, 86% of CMF at full dose, 23% delay  </t>
     </r>
@@ -693,6 +702,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>That paragraph is very confusing ??</t>
     </r>
@@ -710,6 +720,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">26% with delay </t>
     </r>
@@ -754,6 +765,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Unclear if the second cancer totals include the heme malignancies </t>
     </r>
@@ -781,6 +793,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>207 for safety</t>
     </r>
@@ -795,6 +808,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 50</t>
     </r>
@@ -819,6 +833,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>200 for safety</t>
     </r>
@@ -842,6 +857,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>50</t>
     </r>
@@ -856,6 +872,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>196 for safety</t>
     </r>
@@ -870,6 +887,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>75</t>
     </r>
@@ -925,6 +943,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>50</t>
     </r>
@@ -942,6 +961,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>25 on D 1 and 25 on D 8)</t>
     </r>
@@ -1017,6 +1037,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>?</t>
     </r>
@@ -1154,6 +1175,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>6</t>
     </r>
@@ -1174,6 +1196,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>1</t>
     </r>
@@ -1286,6 +1309,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>&amp; N9831</t>
     </r>
@@ -1307,6 +1331,7 @@
         <sz val="9"/>
         <color indexed="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>&amp;N9831</t>
     </r>
@@ -5075,17 +5100,20 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -6396,27 +6424,219 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -6426,215 +6646,23 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6949,17 +6977,17 @@
   <dimension ref="A1:AI99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="K81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J87" sqref="J87"/>
+      <selection pane="bottomRight" activeCell="A84" sqref="A84:XFD87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="78" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="74" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="74" customWidth="1"/>
     <col min="4" max="5" width="10.42578125" style="74" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" style="189" customWidth="1"/>
     <col min="7" max="8" width="16.7109375" style="189" customWidth="1"/>
@@ -6996,41 +7024,41 @@
       <c r="F1" s="181"/>
       <c r="G1" s="181"/>
       <c r="H1" s="181"/>
-      <c r="I1" s="400"/>
+      <c r="I1" s="337"/>
       <c r="J1" s="84"/>
-      <c r="K1" s="371" t="s">
+      <c r="K1" s="369" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="371"/>
-      <c r="M1" s="371"/>
-      <c r="N1" s="371"/>
-      <c r="O1" s="369" t="s">
+      <c r="L1" s="369"/>
+      <c r="M1" s="369"/>
+      <c r="N1" s="369"/>
+      <c r="O1" s="367" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="370"/>
-      <c r="Q1" s="370"/>
-      <c r="R1" s="372" t="s">
+      <c r="P1" s="368"/>
+      <c r="Q1" s="368"/>
+      <c r="R1" s="370" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="372"/>
-      <c r="T1" s="372"/>
-      <c r="U1" s="372"/>
-      <c r="V1" s="373" t="s">
+      <c r="S1" s="370"/>
+      <c r="T1" s="370"/>
+      <c r="U1" s="370"/>
+      <c r="V1" s="371" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="374"/>
-      <c r="X1" s="374"/>
+      <c r="W1" s="372"/>
+      <c r="X1" s="372"/>
       <c r="Y1" s="173"/>
-      <c r="Z1" s="347" t="s">
+      <c r="Z1" s="402" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="347"/>
-      <c r="AB1" s="347"/>
-      <c r="AC1" s="347"/>
-      <c r="AD1" s="347"/>
-      <c r="AE1" s="347"/>
-      <c r="AF1" s="347"/>
-      <c r="AG1" s="347"/>
+      <c r="AA1" s="402"/>
+      <c r="AB1" s="402"/>
+      <c r="AC1" s="402"/>
+      <c r="AD1" s="402"/>
+      <c r="AE1" s="402"/>
+      <c r="AF1" s="402"/>
+      <c r="AG1" s="402"/>
       <c r="AH1" s="172"/>
     </row>
     <row r="2" spans="1:34" s="18" customFormat="1" ht="48.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -7160,7 +7188,7 @@
         <v>734</v>
       </c>
       <c r="H3" s="313"/>
-      <c r="I3" s="401">
+      <c r="I3" s="338">
         <v>26.2</v>
       </c>
       <c r="J3" s="98" t="s">
@@ -7248,7 +7276,7 @@
         <v>728</v>
       </c>
       <c r="H4" s="314"/>
-      <c r="I4" s="402">
+      <c r="I4" s="339">
         <v>26.2</v>
       </c>
       <c r="J4" s="67" t="s">
@@ -7334,7 +7362,7 @@
         <v>732</v>
       </c>
       <c r="H5" s="315"/>
-      <c r="I5" s="403">
+      <c r="I5" s="340">
         <v>26.2</v>
       </c>
       <c r="J5" s="125" t="s">
@@ -7404,7 +7432,7 @@
         <v>112</v>
       </c>
       <c r="H6" s="313"/>
-      <c r="I6" s="401">
+      <c r="I6" s="338">
         <f>15.9*12</f>
         <v>190.8</v>
       </c>
@@ -7475,7 +7503,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="316"/>
-      <c r="I7" s="404">
+      <c r="I7" s="341">
         <v>190.8</v>
       </c>
       <c r="J7" s="125" t="s">
@@ -7567,7 +7595,7 @@
         <v>849</v>
       </c>
       <c r="H8" s="317"/>
-      <c r="I8" s="405">
+      <c r="I8" s="342">
         <v>55.2</v>
       </c>
       <c r="J8" s="30" t="s">
@@ -7653,7 +7681,7 @@
         <v>847</v>
       </c>
       <c r="H9" s="318"/>
-      <c r="I9" s="406">
+      <c r="I9" s="343">
         <v>55.2</v>
       </c>
       <c r="J9" s="308" t="s">
@@ -7739,7 +7767,7 @@
         <v>849</v>
       </c>
       <c r="H10" s="319"/>
-      <c r="I10" s="407">
+      <c r="I10" s="344">
         <v>55.2</v>
       </c>
       <c r="J10" s="32" t="s">
@@ -7825,7 +7853,7 @@
         <v>251</v>
       </c>
       <c r="H11" s="317"/>
-      <c r="I11" s="405">
+      <c r="I11" s="342">
         <v>38.299999999999997</v>
       </c>
       <c r="J11" s="229" t="s">
@@ -7895,44 +7923,44 @@
       </c>
     </row>
     <row r="12" spans="1:34" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="381">
+      <c r="A12" s="364">
         <v>970</v>
       </c>
-      <c r="B12" s="383" t="s">
+      <c r="B12" s="366" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="383" t="s">
+      <c r="C12" s="366" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="383" t="s">
+      <c r="D12" s="366" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="385">
+      <c r="E12" s="354">
         <v>2</v>
       </c>
-      <c r="F12" s="387">
+      <c r="F12" s="352">
         <v>274</v>
       </c>
-      <c r="G12" s="385">
+      <c r="G12" s="354">
         <v>274</v>
       </c>
       <c r="H12" s="320"/>
-      <c r="I12" s="408">
+      <c r="I12" s="362">
         <v>38.299999999999997</v>
       </c>
-      <c r="J12" s="393" t="s">
+      <c r="J12" s="360" t="s">
         <v>74</v>
       </c>
-      <c r="K12" s="389" t="s">
+      <c r="K12" s="356" t="s">
         <v>64</v>
       </c>
-      <c r="L12" s="391">
+      <c r="L12" s="358">
         <v>60</v>
       </c>
-      <c r="M12" s="391">
+      <c r="M12" s="358">
         <v>21</v>
       </c>
-      <c r="N12" s="375">
+      <c r="N12" s="373">
         <v>3</v>
       </c>
       <c r="O12" s="92">
@@ -7944,55 +7972,55 @@
       <c r="Q12" s="92">
         <v>2</v>
       </c>
-      <c r="R12" s="377"/>
-      <c r="S12" s="377"/>
-      <c r="T12" s="377"/>
-      <c r="U12" s="377"/>
-      <c r="V12" s="379"/>
-      <c r="W12" s="379"/>
-      <c r="X12" s="379"/>
-      <c r="Y12" s="355" t="s">
+      <c r="R12" s="375"/>
+      <c r="S12" s="375"/>
+      <c r="T12" s="375"/>
+      <c r="U12" s="375"/>
+      <c r="V12" s="377"/>
+      <c r="W12" s="377"/>
+      <c r="X12" s="377"/>
+      <c r="Y12" s="383" t="s">
         <v>75</v>
       </c>
-      <c r="Z12" s="341">
+      <c r="Z12" s="393">
         <v>0</v>
       </c>
-      <c r="AA12" s="341">
+      <c r="AA12" s="393">
         <v>0</v>
       </c>
-      <c r="AB12" s="341" t="s">
+      <c r="AB12" s="393" t="s">
         <v>38</v>
       </c>
-      <c r="AC12" s="365">
+      <c r="AC12" s="395">
         <v>1</v>
       </c>
-      <c r="AD12" s="359" t="s">
+      <c r="AD12" s="387" t="s">
         <v>76</v>
       </c>
-      <c r="AE12" s="361">
+      <c r="AE12" s="389">
         <v>0</v>
       </c>
-      <c r="AF12" s="363">
+      <c r="AF12" s="391">
         <v>0</v>
       </c>
-      <c r="AG12" s="357"/>
+      <c r="AG12" s="385"/>
       <c r="AH12" s="170"/>
     </row>
     <row r="13" spans="1:34" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="382"/>
-      <c r="B13" s="384"/>
-      <c r="C13" s="384"/>
-      <c r="D13" s="384"/>
-      <c r="E13" s="386"/>
-      <c r="F13" s="388"/>
-      <c r="G13" s="386"/>
+      <c r="A13" s="365"/>
+      <c r="B13" s="361"/>
+      <c r="C13" s="361"/>
+      <c r="D13" s="361"/>
+      <c r="E13" s="355"/>
+      <c r="F13" s="353"/>
+      <c r="G13" s="355"/>
       <c r="H13" s="321"/>
-      <c r="I13" s="409"/>
-      <c r="J13" s="384"/>
-      <c r="K13" s="390"/>
-      <c r="L13" s="392"/>
-      <c r="M13" s="392"/>
-      <c r="N13" s="376"/>
+      <c r="I13" s="363"/>
+      <c r="J13" s="361"/>
+      <c r="K13" s="357"/>
+      <c r="L13" s="359"/>
+      <c r="M13" s="359"/>
+      <c r="N13" s="374"/>
       <c r="O13" s="146">
         <v>1200</v>
       </c>
@@ -8002,22 +8030,22 @@
       <c r="Q13" s="146">
         <v>1</v>
       </c>
-      <c r="R13" s="378"/>
-      <c r="S13" s="378"/>
-      <c r="T13" s="378"/>
-      <c r="U13" s="378"/>
-      <c r="V13" s="380"/>
-      <c r="W13" s="380"/>
-      <c r="X13" s="380"/>
-      <c r="Y13" s="356"/>
-      <c r="Z13" s="342"/>
-      <c r="AA13" s="342"/>
-      <c r="AB13" s="342"/>
-      <c r="AC13" s="366"/>
-      <c r="AD13" s="360"/>
-      <c r="AE13" s="362"/>
-      <c r="AF13" s="364"/>
-      <c r="AG13" s="358"/>
+      <c r="R13" s="376"/>
+      <c r="S13" s="376"/>
+      <c r="T13" s="376"/>
+      <c r="U13" s="376"/>
+      <c r="V13" s="378"/>
+      <c r="W13" s="378"/>
+      <c r="X13" s="378"/>
+      <c r="Y13" s="384"/>
+      <c r="Z13" s="394"/>
+      <c r="AA13" s="394"/>
+      <c r="AB13" s="394"/>
+      <c r="AC13" s="396"/>
+      <c r="AD13" s="388"/>
+      <c r="AE13" s="390"/>
+      <c r="AF13" s="392"/>
+      <c r="AG13" s="386"/>
       <c r="AH13" s="171"/>
     </row>
     <row r="14" spans="1:34" s="16" customFormat="1" ht="36" x14ac:dyDescent="0.25">
@@ -8041,7 +8069,7 @@
         <v>255</v>
       </c>
       <c r="H14" s="322"/>
-      <c r="I14" s="410" t="s">
+      <c r="I14" s="345" t="s">
         <v>761</v>
       </c>
       <c r="J14" s="42" t="s">
@@ -8111,7 +8139,7 @@
         <v>267</v>
       </c>
       <c r="H15" s="323"/>
-      <c r="I15" s="411" t="s">
+      <c r="I15" s="346" t="s">
         <v>761</v>
       </c>
       <c r="J15" s="279" t="s">
@@ -8191,7 +8219,7 @@
         <v>255</v>
       </c>
       <c r="H16" s="324"/>
-      <c r="I16" s="412" t="s">
+      <c r="I16" s="347" t="s">
         <v>761</v>
       </c>
       <c r="J16" s="43" t="s">
@@ -8271,7 +8299,7 @@
         <v>484</v>
       </c>
       <c r="H17" s="322"/>
-      <c r="I17" s="410">
+      <c r="I17" s="345">
         <v>36</v>
       </c>
       <c r="J17" s="42" t="s">
@@ -8357,7 +8385,7 @@
         <v>493</v>
       </c>
       <c r="H18" s="323"/>
-      <c r="I18" s="411">
+      <c r="I18" s="346">
         <v>36</v>
       </c>
       <c r="J18" s="279" t="s">
@@ -8445,7 +8473,7 @@
         <v>501</v>
       </c>
       <c r="H19" s="323"/>
-      <c r="I19" s="411">
+      <c r="I19" s="346">
         <v>36</v>
       </c>
       <c r="J19" s="279" t="s">
@@ -8531,7 +8559,7 @@
         <v>495</v>
       </c>
       <c r="H20" s="324"/>
-      <c r="I20" s="412">
+      <c r="I20" s="347">
         <v>36</v>
       </c>
       <c r="J20" s="43" t="s">
@@ -8617,7 +8645,7 @@
         <v>604</v>
       </c>
       <c r="H21" s="317"/>
-      <c r="I21" s="405">
+      <c r="I21" s="342">
         <v>124.8</v>
       </c>
       <c r="J21" s="30" t="s">
@@ -8699,7 +8727,7 @@
         <v>610</v>
       </c>
       <c r="H22" s="319"/>
-      <c r="I22" s="407">
+      <c r="I22" s="344">
         <v>124.8</v>
       </c>
       <c r="J22" s="32" t="s">
@@ -8781,7 +8809,7 @@
         <v>481</v>
       </c>
       <c r="H23" s="317"/>
-      <c r="I23" s="405">
+      <c r="I23" s="342">
         <v>62.5</v>
       </c>
       <c r="J23" s="30" t="s">
@@ -8851,7 +8879,7 @@
         <v>847</v>
       </c>
       <c r="H24" s="325"/>
-      <c r="I24" s="413">
+      <c r="I24" s="348">
         <v>62.5</v>
       </c>
       <c r="J24" s="309" t="s">
@@ -8927,7 +8955,7 @@
         <v>960</v>
       </c>
       <c r="H25" s="325"/>
-      <c r="I25" s="413">
+      <c r="I25" s="348">
         <v>62.5</v>
       </c>
       <c r="J25" s="309" t="s">
@@ -9005,7 +9033,7 @@
         <v>959</v>
       </c>
       <c r="H26" s="319"/>
-      <c r="I26" s="407">
+      <c r="I26" s="344">
         <v>62.5</v>
       </c>
       <c r="J26" s="32" t="s">
@@ -9083,7 +9111,7 @@
         <v>1441</v>
       </c>
       <c r="H27" s="317"/>
-      <c r="I27" s="405">
+      <c r="I27" s="342">
         <v>79.5</v>
       </c>
       <c r="J27" s="30" t="s">
@@ -9159,7 +9187,7 @@
         <v>1441</v>
       </c>
       <c r="H28" s="319"/>
-      <c r="I28" s="407">
+      <c r="I28" s="344">
         <v>79.5</v>
       </c>
       <c r="J28" s="32" t="s">
@@ -9235,7 +9263,7 @@
         <v>539</v>
       </c>
       <c r="H29" s="317"/>
-      <c r="I29" s="405">
+      <c r="I29" s="342">
         <v>77</v>
       </c>
       <c r="J29" s="30" t="s">
@@ -9323,7 +9351,7 @@
         <v>521</v>
       </c>
       <c r="H30" s="319"/>
-      <c r="I30" s="407">
+      <c r="I30" s="344">
         <v>77</v>
       </c>
       <c r="J30" s="32" t="s">
@@ -9409,7 +9437,7 @@
         <v>360</v>
       </c>
       <c r="H31" s="326"/>
-      <c r="I31" s="414">
+      <c r="I31" s="349">
         <v>64</v>
       </c>
       <c r="J31" s="30" t="s">
@@ -9491,7 +9519,7 @@
         <v>368</v>
       </c>
       <c r="H32" s="319"/>
-      <c r="I32" s="407">
+      <c r="I32" s="344">
         <v>64</v>
       </c>
       <c r="J32" s="32" t="s">
@@ -9575,7 +9603,7 @@
         <v>1551</v>
       </c>
       <c r="H33" s="317"/>
-      <c r="I33" s="405">
+      <c r="I33" s="342">
         <v>69</v>
       </c>
       <c r="J33" s="30" t="s">
@@ -9609,7 +9637,7 @@
       <c r="V33" s="200"/>
       <c r="W33" s="200"/>
       <c r="X33" s="200"/>
-      <c r="Y33" s="367" t="s">
+      <c r="Y33" s="397" t="s">
         <v>134</v>
       </c>
       <c r="Z33" s="10">
@@ -9657,7 +9685,7 @@
         <v>1570</v>
       </c>
       <c r="H34" s="319"/>
-      <c r="I34" s="407">
+      <c r="I34" s="344">
         <v>69</v>
       </c>
       <c r="J34" s="32" t="s">
@@ -9697,7 +9725,7 @@
       <c r="V34" s="201"/>
       <c r="W34" s="201"/>
       <c r="X34" s="201"/>
-      <c r="Y34" s="356"/>
+      <c r="Y34" s="384"/>
       <c r="Z34" s="14">
         <v>4</v>
       </c>
@@ -9741,7 +9769,7 @@
         <v>297</v>
       </c>
       <c r="H35" s="317"/>
-      <c r="I35" s="405">
+      <c r="I35" s="342">
         <v>62</v>
       </c>
       <c r="J35" s="30" t="s">
@@ -9821,7 +9849,7 @@
         <v>290</v>
       </c>
       <c r="H36" s="319"/>
-      <c r="I36" s="407">
+      <c r="I36" s="344">
         <v>62</v>
       </c>
       <c r="J36" s="32" t="s">
@@ -9895,7 +9923,7 @@
         <v>1528</v>
       </c>
       <c r="H37" s="317"/>
-      <c r="I37" s="405">
+      <c r="I37" s="342">
         <v>65</v>
       </c>
       <c r="J37" s="30" t="s">
@@ -9981,7 +10009,7 @@
         <v>1531</v>
       </c>
       <c r="H38" s="319"/>
-      <c r="I38" s="407">
+      <c r="I38" s="344">
         <v>65</v>
       </c>
       <c r="J38" s="32" t="s">
@@ -10073,7 +10101,7 @@
         <v>996</v>
       </c>
       <c r="H39" s="317"/>
-      <c r="I39" s="405">
+      <c r="I39" s="342">
         <v>60</v>
       </c>
       <c r="J39" s="30" t="s">
@@ -10165,7 +10193,7 @@
         <v>1003</v>
       </c>
       <c r="H40" s="319"/>
-      <c r="I40" s="407">
+      <c r="I40" s="344">
         <v>60</v>
       </c>
       <c r="J40" s="32" t="s">
@@ -10263,7 +10291,7 @@
         <v>156</v>
       </c>
       <c r="H41" s="317"/>
-      <c r="I41" s="405">
+      <c r="I41" s="342">
         <v>131</v>
       </c>
       <c r="J41" s="30" t="s">
@@ -10353,7 +10381,7 @@
         <v>161</v>
       </c>
       <c r="H42" s="325"/>
-      <c r="I42" s="413">
+      <c r="I42" s="348">
         <v>131</v>
       </c>
       <c r="J42" s="256" t="s">
@@ -10439,7 +10467,7 @@
         <v>163</v>
       </c>
       <c r="H43" s="319"/>
-      <c r="I43" s="407">
+      <c r="I43" s="344">
         <v>131</v>
       </c>
       <c r="J43" s="32" t="s">
@@ -10525,7 +10553,7 @@
         <v>155</v>
       </c>
       <c r="H44" s="317"/>
-      <c r="I44" s="405">
+      <c r="I44" s="342">
         <v>72</v>
       </c>
       <c r="J44" s="30" t="s">
@@ -10595,7 +10623,7 @@
         <v>163</v>
       </c>
       <c r="H45" s="319"/>
-      <c r="I45" s="407">
+      <c r="I45" s="344">
         <v>72</v>
       </c>
       <c r="J45" s="32" t="s">
@@ -10675,7 +10703,7 @@
         <v>235</v>
       </c>
       <c r="H46" s="317"/>
-      <c r="I46" s="405">
+      <c r="I46" s="342">
         <v>78</v>
       </c>
       <c r="J46" s="30" t="s">
@@ -10767,7 +10795,7 @@
         <v>236</v>
       </c>
       <c r="H47" s="319"/>
-      <c r="I47" s="407">
+      <c r="I47" s="344">
         <v>78</v>
       </c>
       <c r="J47" s="32" t="s">
@@ -10847,7 +10875,7 @@
         <v>303</v>
       </c>
       <c r="H48" s="317"/>
-      <c r="I48" s="405">
+      <c r="I48" s="342">
         <v>57.6</v>
       </c>
       <c r="J48" s="30" t="s">
@@ -10927,7 +10955,7 @@
         <v>301</v>
       </c>
       <c r="H49" s="319"/>
-      <c r="I49" s="407">
+      <c r="I49" s="344">
         <v>57.6</v>
       </c>
       <c r="J49" s="32" t="s">
@@ -10999,7 +11027,7 @@
         <v>180</v>
       </c>
       <c r="H50" s="317"/>
-      <c r="I50" s="405">
+      <c r="I50" s="342">
         <v>58</v>
       </c>
       <c r="J50" s="30" t="s">
@@ -11022,24 +11050,24 @@
       <c r="Y50" s="300" t="s">
         <v>186</v>
       </c>
-      <c r="Z50" s="351" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA50" s="351" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB50" s="368" t="s">
+      <c r="Z50" s="398" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA50" s="398" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB50" s="400" t="s">
         <v>38</v>
       </c>
-      <c r="AC50" s="348">
+      <c r="AC50" s="403">
         <v>4</v>
       </c>
-      <c r="AD50" s="349" t="s">
+      <c r="AD50" s="405" t="s">
         <v>187</v>
       </c>
-      <c r="AE50" s="351"/>
-      <c r="AF50" s="351"/>
-      <c r="AG50" s="352"/>
+      <c r="AE50" s="398"/>
+      <c r="AF50" s="398"/>
+      <c r="AG50" s="379"/>
       <c r="AH50" s="168" t="s">
         <v>188</v>
       </c>
@@ -11067,7 +11095,7 @@
         <v>199</v>
       </c>
       <c r="H51" s="325"/>
-      <c r="I51" s="413">
+      <c r="I51" s="348">
         <v>58</v>
       </c>
       <c r="J51" s="309" t="s">
@@ -11090,14 +11118,14 @@
       <c r="Y51" s="290" t="s">
         <v>189</v>
       </c>
-      <c r="Z51" s="337"/>
-      <c r="AA51" s="337"/>
-      <c r="AB51" s="341"/>
-      <c r="AC51" s="343"/>
-      <c r="AD51" s="350"/>
-      <c r="AE51" s="337"/>
-      <c r="AF51" s="337"/>
-      <c r="AG51" s="339"/>
+      <c r="Z51" s="399"/>
+      <c r="AA51" s="399"/>
+      <c r="AB51" s="393"/>
+      <c r="AC51" s="404"/>
+      <c r="AD51" s="406"/>
+      <c r="AE51" s="399"/>
+      <c r="AF51" s="399"/>
+      <c r="AG51" s="380"/>
       <c r="AH51" s="168"/>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.25">
@@ -11123,7 +11151,7 @@
         <v>180</v>
       </c>
       <c r="H52" s="325"/>
-      <c r="I52" s="413">
+      <c r="I52" s="348">
         <v>58</v>
       </c>
       <c r="J52" s="309" t="s">
@@ -11164,24 +11192,24 @@
         <v>8</v>
       </c>
       <c r="Y52" s="290"/>
-      <c r="Z52" s="337" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA52" s="337" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB52" s="341" t="s">
+      <c r="Z52" s="399" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA52" s="399" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB52" s="393" t="s">
         <v>38</v>
       </c>
-      <c r="AC52" s="343">
+      <c r="AC52" s="404">
         <v>2</v>
       </c>
-      <c r="AD52" s="345" t="s">
+      <c r="AD52" s="409" t="s">
         <v>190</v>
       </c>
-      <c r="AE52" s="337"/>
-      <c r="AF52" s="337"/>
-      <c r="AG52" s="339"/>
+      <c r="AE52" s="399"/>
+      <c r="AF52" s="399"/>
+      <c r="AG52" s="380"/>
       <c r="AH52" s="168"/>
     </row>
     <row r="53" spans="1:34" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11207,7 +11235,7 @@
         <v>200</v>
       </c>
       <c r="H53" s="319"/>
-      <c r="I53" s="407">
+      <c r="I53" s="344">
         <v>58</v>
       </c>
       <c r="J53" s="32" t="s">
@@ -11250,14 +11278,14 @@
       <c r="Y53" s="291" t="s">
         <v>191</v>
       </c>
-      <c r="Z53" s="338"/>
-      <c r="AA53" s="338"/>
-      <c r="AB53" s="342"/>
-      <c r="AC53" s="344"/>
-      <c r="AD53" s="346"/>
-      <c r="AE53" s="338"/>
-      <c r="AF53" s="338"/>
-      <c r="AG53" s="340"/>
+      <c r="Z53" s="401"/>
+      <c r="AA53" s="401"/>
+      <c r="AB53" s="394"/>
+      <c r="AC53" s="408"/>
+      <c r="AD53" s="410"/>
+      <c r="AE53" s="401"/>
+      <c r="AF53" s="401"/>
+      <c r="AG53" s="407"/>
       <c r="AH53" s="169"/>
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.25">
@@ -11283,7 +11311,7 @@
         <v>767</v>
       </c>
       <c r="H54" s="317"/>
-      <c r="I54" s="405">
+      <c r="I54" s="342">
         <v>69.3</v>
       </c>
       <c r="J54" s="30" t="s">
@@ -11367,7 +11395,7 @@
         <v>763</v>
       </c>
       <c r="H55" s="325"/>
-      <c r="I55" s="413">
+      <c r="I55" s="348">
         <v>69.3</v>
       </c>
       <c r="J55" s="309" t="s">
@@ -11449,7 +11477,7 @@
         <v>771</v>
       </c>
       <c r="H56" s="319"/>
-      <c r="I56" s="407">
+      <c r="I56" s="344">
         <v>69.3</v>
       </c>
       <c r="J56" s="32" t="s">
@@ -11531,7 +11559,7 @@
         <v>745</v>
       </c>
       <c r="H57" s="317"/>
-      <c r="I57" s="405">
+      <c r="I57" s="342">
         <v>124</v>
       </c>
       <c r="J57" s="30" t="s">
@@ -11619,7 +11647,7 @@
         <v>746</v>
       </c>
       <c r="H58" s="319"/>
-      <c r="I58" s="407">
+      <c r="I58" s="344">
         <v>124</v>
       </c>
       <c r="J58" s="32" t="s">
@@ -11707,7 +11735,7 @@
         <v>751</v>
       </c>
       <c r="H59" s="317"/>
-      <c r="I59" s="405">
+      <c r="I59" s="342">
         <v>59</v>
       </c>
       <c r="J59" s="30" t="s">
@@ -11803,7 +11831,7 @@
         <v>745</v>
       </c>
       <c r="H60" s="319"/>
-      <c r="I60" s="407">
+      <c r="I60" s="344">
         <v>59</v>
       </c>
       <c r="J60" s="32" t="s">
@@ -11901,7 +11929,7 @@
         <v>1590</v>
       </c>
       <c r="H61" s="327"/>
-      <c r="I61" s="415">
+      <c r="I61" s="350">
         <f>7.2*12</f>
         <v>86.4</v>
       </c>
@@ -11982,7 +12010,7 @@
         <v>1524</v>
       </c>
       <c r="H62" s="328"/>
-      <c r="I62" s="416">
+      <c r="I62" s="351">
         <v>86.4</v>
       </c>
       <c r="J62" s="33" t="s">
@@ -12064,7 +12092,7 @@
         <v>271</v>
       </c>
       <c r="H63" s="317"/>
-      <c r="I63" s="405">
+      <c r="I63" s="342">
         <v>110</v>
       </c>
       <c r="J63" s="30" t="s">
@@ -12154,7 +12182,7 @@
         <v>266</v>
       </c>
       <c r="H64" s="319"/>
-      <c r="I64" s="407">
+      <c r="I64" s="344">
         <v>110</v>
       </c>
       <c r="J64" s="32" t="s">
@@ -12244,7 +12272,7 @@
         <v>171</v>
       </c>
       <c r="H65" s="317"/>
-      <c r="I65" s="405">
+      <c r="I65" s="342">
         <f>8.3*12</f>
         <v>99.600000000000009</v>
       </c>
@@ -12333,7 +12361,7 @@
         <v>173</v>
       </c>
       <c r="H66" s="319"/>
-      <c r="I66" s="407">
+      <c r="I66" s="344">
         <v>99.6</v>
       </c>
       <c r="J66" s="32" t="s">
@@ -12417,7 +12445,7 @@
         <v>1649</v>
       </c>
       <c r="H67" s="317"/>
-      <c r="I67" s="405">
+      <c r="I67" s="342">
         <v>65</v>
       </c>
       <c r="J67" s="30" t="s">
@@ -12505,7 +12533,7 @@
         <v>1649</v>
       </c>
       <c r="H68" s="319"/>
-      <c r="I68" s="407">
+      <c r="I68" s="344">
         <v>65</v>
       </c>
       <c r="J68" s="32" t="s">
@@ -12591,7 +12619,7 @@
         <v>498</v>
       </c>
       <c r="H69" s="317"/>
-      <c r="I69" s="405">
+      <c r="I69" s="342">
         <v>60</v>
       </c>
       <c r="J69" s="30" t="s">
@@ -12653,7 +12681,7 @@
         <v>496</v>
       </c>
       <c r="H70" s="325"/>
-      <c r="I70" s="413">
+      <c r="I70" s="348">
         <v>60</v>
       </c>
       <c r="J70" s="309" t="s">
@@ -12713,7 +12741,7 @@
         <v>494</v>
       </c>
       <c r="H71" s="325"/>
-      <c r="I71" s="413">
+      <c r="I71" s="348">
         <v>60</v>
       </c>
       <c r="J71" s="309" t="s">
@@ -12785,7 +12813,7 @@
         <v>494</v>
       </c>
       <c r="H72" s="319"/>
-      <c r="I72" s="407">
+      <c r="I72" s="344">
         <v>60</v>
       </c>
       <c r="J72" s="32" t="s">
@@ -12859,7 +12887,7 @@
         <v>951</v>
       </c>
       <c r="H73" s="317"/>
-      <c r="I73" s="405">
+      <c r="I73" s="342">
         <v>63.3</v>
       </c>
       <c r="J73" s="30" t="s">
@@ -12955,7 +12983,7 @@
         <v>974</v>
       </c>
       <c r="H74" s="319"/>
-      <c r="I74" s="407">
+      <c r="I74" s="344">
         <v>63.3</v>
       </c>
       <c r="J74" s="32" t="s">
@@ -13043,7 +13071,7 @@
         <v>271</v>
       </c>
       <c r="H75" s="317"/>
-      <c r="I75" s="405">
+      <c r="I75" s="342">
         <v>70</v>
       </c>
       <c r="J75" s="30" t="s">
@@ -13133,7 +13161,7 @@
         <v>265</v>
       </c>
       <c r="H76" s="319"/>
-      <c r="I76" s="407">
+      <c r="I76" s="344">
         <v>70</v>
       </c>
       <c r="J76" s="32" t="s">
@@ -13219,7 +13247,7 @@
         <v>163</v>
       </c>
       <c r="H77" s="317"/>
-      <c r="I77" s="405">
+      <c r="I77" s="342">
         <v>83</v>
       </c>
       <c r="J77" s="30" t="s">
@@ -13289,7 +13317,7 @@
         <v>168</v>
       </c>
       <c r="H78" s="319"/>
-      <c r="I78" s="407">
+      <c r="I78" s="344">
         <v>83</v>
       </c>
       <c r="J78" s="32" t="s">
@@ -13373,7 +13401,7 @@
       <c r="F79" s="182"/>
       <c r="G79" s="182"/>
       <c r="H79" s="317"/>
-      <c r="I79" s="405"/>
+      <c r="I79" s="342"/>
       <c r="J79" s="30" t="s">
         <v>96</v>
       </c>
@@ -13421,7 +13449,7 @@
       <c r="F80" s="186"/>
       <c r="G80" s="186"/>
       <c r="H80" s="325"/>
-      <c r="I80" s="413"/>
+      <c r="I80" s="348"/>
       <c r="J80" s="309" t="s">
         <v>255</v>
       </c>
@@ -13469,7 +13497,7 @@
       <c r="F81" s="184"/>
       <c r="G81" s="184"/>
       <c r="H81" s="319"/>
-      <c r="I81" s="407"/>
+      <c r="I81" s="344"/>
       <c r="J81" s="32" t="s">
         <v>256</v>
       </c>
@@ -13521,7 +13549,7 @@
         <v>872</v>
       </c>
       <c r="H82" s="317"/>
-      <c r="I82" s="405">
+      <c r="I82" s="342">
         <f>2.4*12</f>
         <v>28.799999999999997</v>
       </c>
@@ -13618,7 +13646,7 @@
         <v>864</v>
       </c>
       <c r="H83" s="319"/>
-      <c r="I83" s="407">
+      <c r="I83" s="344">
         <v>28.8</v>
       </c>
       <c r="J83" s="32" t="s">
@@ -13712,7 +13740,7 @@
         <v>1107</v>
       </c>
       <c r="H84" s="317"/>
-      <c r="I84" s="405">
+      <c r="I84" s="342">
         <v>73.2</v>
       </c>
       <c r="J84" s="30" t="s">
@@ -13765,10 +13793,10 @@
       <c r="AE84" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="AF84" s="353" t="s">
+      <c r="AF84" s="381" t="s">
         <v>71</v>
       </c>
-      <c r="AG84" s="352">
+      <c r="AG84" s="379">
         <v>7</v>
       </c>
       <c r="AH84" s="168" t="s">
@@ -13798,7 +13826,7 @@
         <v>766</v>
       </c>
       <c r="H85" s="325"/>
-      <c r="I85" s="413">
+      <c r="I85" s="348">
         <v>73.2</v>
       </c>
       <c r="J85" s="309" t="s">
@@ -13851,8 +13879,8 @@
       <c r="AE85" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="AF85" s="354"/>
-      <c r="AG85" s="339"/>
+      <c r="AF85" s="382"/>
+      <c r="AG85" s="380"/>
       <c r="AH85" s="168"/>
     </row>
     <row r="86" spans="1:34" ht="36" x14ac:dyDescent="0.25">
@@ -13878,7 +13906,7 @@
         <v>1119</v>
       </c>
       <c r="H86" s="325"/>
-      <c r="I86" s="413">
+      <c r="I86" s="348">
         <v>73.2</v>
       </c>
       <c r="J86" s="309" t="s">
@@ -13956,7 +13984,7 @@
         <v>782</v>
       </c>
       <c r="H87" s="319"/>
-      <c r="I87" s="407">
+      <c r="I87" s="344">
         <v>73.2</v>
       </c>
       <c r="J87" s="32" t="s">
@@ -14034,7 +14062,7 @@
         <v>1617</v>
       </c>
       <c r="H88" s="317"/>
-      <c r="I88" s="405">
+      <c r="I88" s="342">
         <v>64</v>
       </c>
       <c r="J88" s="30" t="s">
@@ -14120,7 +14148,7 @@
         <v>1624</v>
       </c>
       <c r="H89" s="325"/>
-      <c r="I89" s="413">
+      <c r="I89" s="348">
         <v>64</v>
       </c>
       <c r="J89" s="309" t="s">
@@ -14204,7 +14232,7 @@
         <v>1618</v>
       </c>
       <c r="H90" s="319"/>
-      <c r="I90" s="407">
+      <c r="I90" s="344">
         <v>64</v>
       </c>
       <c r="J90" s="32" t="s">
@@ -14288,7 +14316,7 @@
         <v>545</v>
       </c>
       <c r="H91" s="317"/>
-      <c r="I91" s="405">
+      <c r="I91" s="342">
         <f>7*12</f>
         <v>84</v>
       </c>
@@ -14381,7 +14409,7 @@
         <v>544</v>
       </c>
       <c r="H92" s="325"/>
-      <c r="I92" s="413">
+      <c r="I92" s="348">
         <v>84</v>
       </c>
       <c r="J92" s="309" t="s">
@@ -14479,7 +14507,7 @@
         <v>502</v>
       </c>
       <c r="H93" s="325"/>
-      <c r="I93" s="413">
+      <c r="I93" s="348">
         <v>84</v>
       </c>
       <c r="J93" s="309" t="s">
@@ -14571,7 +14599,7 @@
         <v>500</v>
       </c>
       <c r="H94" s="319"/>
-      <c r="I94" s="407">
+      <c r="I94" s="344">
         <v>84</v>
       </c>
       <c r="J94" s="32" t="s">
@@ -14669,7 +14697,7 @@
         <v>978</v>
       </c>
       <c r="H95" s="317"/>
-      <c r="I95" s="405">
+      <c r="I95" s="342">
         <v>59</v>
       </c>
       <c r="J95" s="30" t="s">
@@ -14753,7 +14781,7 @@
         <v>795</v>
       </c>
       <c r="H96" s="325"/>
-      <c r="I96" s="413">
+      <c r="I96" s="348">
         <v>59</v>
       </c>
       <c r="J96" s="309" t="s">
@@ -14833,7 +14861,7 @@
         <v>177</v>
       </c>
       <c r="H97" s="319"/>
-      <c r="I97" s="407">
+      <c r="I97" s="344">
         <v>59</v>
       </c>
       <c r="J97" s="32" t="s">
@@ -14897,7 +14925,7 @@
         <v>751</v>
       </c>
       <c r="H98" s="317"/>
-      <c r="I98" s="405">
+      <c r="I98" s="342">
         <f>12*9</f>
         <v>108</v>
       </c>
@@ -14985,7 +15013,7 @@
         <v>742</v>
       </c>
       <c r="H99" s="319"/>
-      <c r="I99" s="407">
+      <c r="I99" s="344">
         <v>108</v>
       </c>
       <c r="J99" s="32" t="s">
@@ -15049,30 +15077,19 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="S12:S13"/>
-    <mergeCell ref="T12:T13"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="V12:V13"/>
-    <mergeCell ref="W12:W13"/>
-    <mergeCell ref="X12:X13"/>
+    <mergeCell ref="AF52:AF53"/>
+    <mergeCell ref="AG52:AG53"/>
+    <mergeCell ref="Z52:Z53"/>
+    <mergeCell ref="AA52:AA53"/>
+    <mergeCell ref="AB52:AB53"/>
+    <mergeCell ref="AC52:AC53"/>
+    <mergeCell ref="AD52:AD53"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="AC50:AC51"/>
+    <mergeCell ref="AD50:AD51"/>
+    <mergeCell ref="AE50:AE51"/>
+    <mergeCell ref="AF50:AF51"/>
+    <mergeCell ref="AG50:AG51"/>
     <mergeCell ref="AG84:AG85"/>
     <mergeCell ref="AF84:AF85"/>
     <mergeCell ref="Y12:Y13"/>
@@ -15089,19 +15106,30 @@
     <mergeCell ref="AA50:AA51"/>
     <mergeCell ref="AB50:AB51"/>
     <mergeCell ref="AE52:AE53"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="AC50:AC51"/>
-    <mergeCell ref="AD50:AD51"/>
-    <mergeCell ref="AE50:AE51"/>
-    <mergeCell ref="AF50:AF51"/>
-    <mergeCell ref="AG50:AG51"/>
-    <mergeCell ref="AF52:AF53"/>
-    <mergeCell ref="AG52:AG53"/>
-    <mergeCell ref="Z52:Z53"/>
-    <mergeCell ref="AA52:AA53"/>
-    <mergeCell ref="AB52:AB53"/>
-    <mergeCell ref="AC52:AC53"/>
-    <mergeCell ref="AD52:AD53"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="S12:S13"/>
+    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="V12:V13"/>
+    <mergeCell ref="W12:W13"/>
+    <mergeCell ref="X12:X13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15628,70 +15656,70 @@
       <c r="Q10" s="212"/>
     </row>
     <row r="11" spans="1:17" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="395">
+      <c r="A11" s="413">
         <v>970</v>
       </c>
-      <c r="B11" s="395" t="s">
+      <c r="B11" s="413" t="s">
         <v>334</v>
       </c>
-      <c r="C11" s="395" t="s">
+      <c r="C11" s="413" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="395" t="s">
+      <c r="D11" s="413" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="395">
+      <c r="E11" s="413">
         <v>2</v>
       </c>
-      <c r="F11" s="394">
+      <c r="F11" s="416">
         <v>274</v>
       </c>
-      <c r="G11" s="395">
+      <c r="G11" s="413">
         <v>274</v>
       </c>
-      <c r="H11" s="397" t="s">
+      <c r="H11" s="412" t="s">
         <v>335</v>
       </c>
-      <c r="I11" s="397" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="397" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="398" t="s">
+      <c r="I11" s="412" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="412" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="414" t="s">
         <v>730</v>
       </c>
-      <c r="L11" s="397" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="396" t="s">
+      <c r="L11" s="412" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="411" t="s">
         <v>339</v>
       </c>
-      <c r="N11" s="396" t="s">
+      <c r="N11" s="411" t="s">
         <v>340</v>
       </c>
-      <c r="O11" s="396" t="s">
+      <c r="O11" s="411" t="s">
         <v>341</v>
       </c>
       <c r="P11" s="212"/>
       <c r="Q11" s="212"/>
     </row>
     <row r="12" spans="1:17" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="395"/>
-      <c r="B12" s="395"/>
-      <c r="C12" s="395"/>
-      <c r="D12" s="395"/>
-      <c r="E12" s="395"/>
-      <c r="F12" s="394"/>
-      <c r="G12" s="395"/>
-      <c r="H12" s="397"/>
-      <c r="I12" s="397"/>
-      <c r="J12" s="397"/>
-      <c r="K12" s="399"/>
-      <c r="L12" s="397"/>
-      <c r="M12" s="397"/>
-      <c r="N12" s="397"/>
-      <c r="O12" s="397"/>
+      <c r="A12" s="413"/>
+      <c r="B12" s="413"/>
+      <c r="C12" s="413"/>
+      <c r="D12" s="413"/>
+      <c r="E12" s="413"/>
+      <c r="F12" s="416"/>
+      <c r="G12" s="413"/>
+      <c r="H12" s="412"/>
+      <c r="I12" s="412"/>
+      <c r="J12" s="412"/>
+      <c r="K12" s="415"/>
+      <c r="L12" s="412"/>
+      <c r="M12" s="412"/>
+      <c r="N12" s="412"/>
+      <c r="O12" s="412"/>
       <c r="P12" s="309"/>
       <c r="Q12" s="309"/>
     </row>
@@ -19478,6 +19506,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="G11:G12"/>
@@ -19487,12 +19521,6 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="K11:K12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>